<commit_message>
Updated file with github reference
</commit_message>
<xml_diff>
--- a/ML Project Governance Framework.xlsx
+++ b/ML Project Governance Framework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Talks\ML Project Governance Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533D5859-C3FB-4EB5-A8D4-A72FC2CD5198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E45DB51-327B-4401-8B84-7166271A1D8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DA3D3E90-2B9F-433A-AD58-1BA421E9C858}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>Reference: https://www.luminovo.ai/</t>
   </si>
@@ -248,12 +248,18 @@
   <si>
     <t xml:space="preserve">ML Project Governance Framework is a framework that can be followed by any new Data Science business or team. It will help in formulating strategies around how to use Data Science as a business, how to architect Data Science based solutions and team formation strategy, typical Data Science project lifecycle components, commonly available Deep Learning toolsets and frameworks and best practices used by Data Scientists. </t>
   </si>
+  <si>
+    <t>https://github.com/indranildchandra/ml-project-governance-framework</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +287,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,10 +332,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -366,8 +381,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,7 +863,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE7B67F-9103-4766-8D42-2CF7AD0C6D34}">
-  <dimension ref="A3:B3"/>
+  <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -865,7 +883,18 @@
         <v>64</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{DCA806E4-5CA6-41F8-8247-242DBD8274C8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>